<commit_message>
Add APK file and update project schedule
Added the Loja-Social.apk file to the apk directory and updated the project schedule spreadsheet (Cronograma.xlsx) in the internal documents. These changes likely reflect a new build and an updated timeline.
</commit_message>
<xml_diff>
--- a/Documentos do Projeto/Documentos Internos/Cronograma.xlsx
+++ b/Documentos do Projeto/Documentos Internos/Cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\GitHub\PDM_PA_50_10\Documentos Internos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\GitHub\PDM_PA_50_10\Documentos do Projeto\Documentos Internos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CDF630-006F-4F44-8225-B2D9FA6121C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5165DCC3-27F7-49ED-87E9-E70B19F7F6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="156">
   <si>
     <t>MÊS</t>
   </si>
@@ -536,30 +536,12 @@
     <t>Sprint 2</t>
   </si>
   <si>
-    <t>PAP-14</t>
-  </si>
-  <si>
-    <t>Preparação do Back-end</t>
-  </si>
-  <si>
-    <t>PAP-23</t>
-  </si>
-  <si>
-    <t>Continuação do Frontend</t>
-  </si>
-  <si>
-    <t>Não atribuída</t>
-  </si>
-  <si>
     <t>Sprint 3</t>
   </si>
   <si>
     <t>PAP-22</t>
   </si>
   <si>
-    <t>Continuação do Backend</t>
-  </si>
-  <si>
     <t>PAP-17</t>
   </si>
   <si>
@@ -569,27 +551,12 @@
     <t>Sprint 4</t>
   </si>
   <si>
-    <t>PAP-16</t>
-  </si>
-  <si>
-    <t>Desenvolvimento de testes unitários</t>
-  </si>
-  <si>
-    <t>PAP-19</t>
-  </si>
-  <si>
-    <t>Debugging no Frontend</t>
-  </si>
-  <si>
     <t>Sprint 5</t>
   </si>
   <si>
     <t>PAP-18</t>
   </si>
   <si>
-    <t>Debugging no Backend</t>
-  </si>
-  <si>
     <t>PAP-28</t>
   </si>
   <si>
@@ -642,6 +609,15 @@
   </si>
   <si>
     <t>Correção dos diagramas</t>
+  </si>
+  <si>
+    <t>Debugging da aplicação</t>
+  </si>
+  <si>
+    <t>Continuação da aplicação</t>
+  </si>
+  <si>
+    <t>Costa e Tierri</t>
   </si>
 </sst>
 </file>
@@ -959,14 +935,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1257,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" zoomScale="104" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="104" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -1279,37 +1255,37 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="30" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="30" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="30" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="30" t="s">
+      <c r="N1" s="29"/>
+      <c r="O1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="31"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="30">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2">
@@ -1345,7 +1321,7 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="60">
-      <c r="A3" s="29"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -1383,7 +1359,7 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" ht="44.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -1419,7 +1395,7 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" ht="82.5" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2">
@@ -1454,7 +1430,7 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="45">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="2">
         <v>7</v>
       </c>
@@ -1489,7 +1465,7 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="29"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -1524,7 +1500,7 @@
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" ht="44.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="2">
         <v>9</v>
       </c>
@@ -1561,7 +1537,7 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="45">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2">
@@ -1599,7 +1575,7 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="29"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="2">
         <v>11</v>
       </c>
@@ -1632,7 +1608,7 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="29"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="2">
         <v>12</v>
       </c>
@@ -1665,7 +1641,7 @@
       <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" ht="45">
-      <c r="A12" s="29"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="2">
         <v>13</v>
       </c>
@@ -1703,7 +1679,7 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" ht="60">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2">
@@ -1742,7 +1718,7 @@
       <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="29"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="2">
         <v>15</v>
       </c>
@@ -1775,7 +1751,7 @@
       <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" ht="45">
-      <c r="A15" s="29"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="2">
         <v>16</v>
       </c>
@@ -1812,7 +1788,7 @@
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="29"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="2">
         <v>17</v>
       </c>
@@ -1846,7 +1822,7 @@
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="29"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="2">
         <v>18</v>
       </c>
@@ -1880,7 +1856,7 @@
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2">
@@ -1918,7 +1894,7 @@
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16" ht="30">
-      <c r="A19" s="29"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="2">
         <v>15</v>
       </c>
@@ -1949,6 +1925,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
@@ -1956,11 +1937,6 @@
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" location="Entregas!A6" display="1ª Entrega / apresentação" xr:uid="{0A4A7E6F-5B19-4043-8AA1-14A479757A24}"/>
@@ -1977,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895AAF2E-62E0-4D99-9699-CE3C7B3F175D}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A37" activeCellId="2" sqref="A33:A35 B36 A37"/>
+    <sheetView topLeftCell="A24" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2127,13 +2103,13 @@
     </row>
     <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="24" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B23" s="17"/>
     </row>
     <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="24" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B24" s="17"/>
     </row>
@@ -2230,25 +2206,25 @@
       <c r="B40" s="22"/>
     </row>
     <row r="41" spans="1:2" ht="15.75">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="17"/>
     </row>
     <row r="42" spans="1:2" ht="15.75">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="24" t="s">
         <v>55</v>
       </c>
       <c r="B42" s="17"/>
     </row>
     <row r="43" spans="1:2" ht="15.75">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="24" t="s">
         <v>56</v>
       </c>
       <c r="B43" s="17"/>
     </row>
     <row r="44" spans="1:2" ht="15.75">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="24" t="s">
         <v>57</v>
       </c>
       <c r="B44" s="17"/>
@@ -2344,10 +2320,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5866E5C1-172E-4782-AFD1-E9BEE95982AD}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2914,7 +2890,9 @@
       <c r="F11" s="27">
         <v>45950.519264664355</v>
       </c>
-      <c r="G11" s="27"/>
+      <c r="G11" s="27">
+        <v>45981</v>
+      </c>
       <c r="H11" s="26" t="s">
         <v>91</v>
       </c>
@@ -2925,7 +2903,7 @@
         <v>93</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="L11" s="26" t="s">
         <v>118</v>
@@ -2957,7 +2935,7 @@
         <v>89</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E12" s="27">
         <v>45940.607197754631</v>
@@ -3054,7 +3032,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>88</v>
@@ -3063,16 +3041,16 @@
         <v>89</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E14" s="27">
-        <v>45950.45394861111</v>
+        <v>45950.457830729167</v>
       </c>
       <c r="F14" s="27">
-        <v>45950.513370104163</v>
+        <v>45950.513444525466</v>
       </c>
       <c r="G14" s="27">
-        <v>45970</v>
+        <v>45981</v>
       </c>
       <c r="H14" s="26" t="s">
         <v>91</v>
@@ -3084,7 +3062,7 @@
         <v>93</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="L14" s="26" t="s">
         <v>127</v>
@@ -3107,7 +3085,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="26" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>88</v>
@@ -3116,16 +3094,16 @@
         <v>89</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="E15" s="27">
-        <v>45950.457830729167</v>
+        <v>45943.431502662039</v>
       </c>
       <c r="F15" s="27">
-        <v>45950.513444525466</v>
+        <v>45950.510677638886</v>
       </c>
       <c r="G15" s="27">
-        <v>45981</v>
+        <v>45989.510682870372</v>
       </c>
       <c r="H15" s="26" t="s">
         <v>91</v>
@@ -3137,7 +3115,7 @@
         <v>93</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="L15" s="26" t="s">
         <v>127</v>
@@ -3158,9 +3136,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" ht="12.75" customHeight="1">
       <c r="A16" s="26" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>88</v>
@@ -3169,16 +3147,16 @@
         <v>89</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E16" s="27">
-        <v>45943.431502662039</v>
+        <v>45950.512106817128</v>
       </c>
       <c r="F16" s="27">
-        <v>45950.510677638886</v>
+        <v>45950.513540092594</v>
       </c>
       <c r="G16" s="27">
-        <v>45989.510682870372</v>
+        <v>46015</v>
       </c>
       <c r="H16" s="26" t="s">
         <v>91</v>
@@ -3187,13 +3165,13 @@
         <v>92</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M16" s="26">
         <v>0</v>
@@ -3213,7 +3191,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>88</v>
@@ -3222,15 +3200,17 @@
         <v>89</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E17" s="27">
-        <v>45950.512106817128</v>
+        <v>45950.506588495373</v>
       </c>
       <c r="F17" s="27">
-        <v>45950.513540092594</v>
-      </c>
-      <c r="G17" s="27"/>
+        <v>45950.506588495373</v>
+      </c>
+      <c r="G17" s="27">
+        <v>46016</v>
+      </c>
       <c r="H17" s="26" t="s">
         <v>91</v>
       </c>
@@ -3241,10 +3221,10 @@
         <v>117</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M17" s="26">
         <v>0</v>
@@ -3264,7 +3244,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="26" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>88</v>
@@ -3273,15 +3253,17 @@
         <v>89</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="E18" s="27">
-        <v>45950.512167835652</v>
+        <v>45950.506925208334</v>
       </c>
       <c r="F18" s="27">
-        <v>45950.51362597222</v>
-      </c>
-      <c r="G18" s="27"/>
+        <v>45950.506925208334</v>
+      </c>
+      <c r="G18" s="27">
+        <v>46017</v>
+      </c>
       <c r="H18" s="26" t="s">
         <v>91</v>
       </c>
@@ -3292,7 +3274,7 @@
         <v>117</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="L18" s="26" t="s">
         <v>133</v>
@@ -3315,7 +3297,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="26" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>88</v>
@@ -3324,15 +3306,17 @@
         <v>89</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E19" s="27">
-        <v>45950.506292314814</v>
+        <v>45950.519731238426</v>
       </c>
       <c r="F19" s="27">
-        <v>45950.506292314814</v>
-      </c>
-      <c r="G19" s="27"/>
+        <v>45950.519731238426</v>
+      </c>
+      <c r="G19" s="27">
+        <v>46030</v>
+      </c>
       <c r="H19" s="26" t="s">
         <v>91</v>
       </c>
@@ -3343,10 +3327,10 @@
         <v>117</v>
       </c>
       <c r="K19" s="26" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M19" s="26">
         <v>0</v>
@@ -3366,7 +3350,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="26" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>88</v>
@@ -3375,15 +3359,17 @@
         <v>89</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E20" s="27">
-        <v>45950.506588495373</v>
+        <v>45950.519979537035</v>
       </c>
       <c r="F20" s="27">
-        <v>45950.506588495373</v>
-      </c>
-      <c r="G20" s="27"/>
+        <v>45950.519979537035</v>
+      </c>
+      <c r="G20" s="27">
+        <v>46031</v>
+      </c>
       <c r="H20" s="26" t="s">
         <v>91</v>
       </c>
@@ -3394,10 +3380,10 @@
         <v>117</v>
       </c>
       <c r="K20" s="26" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M20" s="26">
         <v>0</v>
@@ -3417,7 +3403,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="26" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>88</v>
@@ -3426,15 +3412,17 @@
         <v>89</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E21" s="27">
-        <v>45950.506925208334</v>
+        <v>45950.520159583335</v>
       </c>
       <c r="F21" s="27">
-        <v>45950.506925208334</v>
-      </c>
-      <c r="G21" s="27"/>
+        <v>45950.520159583335</v>
+      </c>
+      <c r="G21" s="27">
+        <v>46032</v>
+      </c>
       <c r="H21" s="26" t="s">
         <v>91</v>
       </c>
@@ -3445,10 +3433,10 @@
         <v>117</v>
       </c>
       <c r="K21" s="26" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M21" s="26">
         <v>0</v>
@@ -3468,7 +3456,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="26" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>88</v>
@@ -3477,15 +3465,17 @@
         <v>89</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E22" s="27">
-        <v>45950.507307974534</v>
+        <v>45950.520298958334</v>
       </c>
       <c r="F22" s="27">
-        <v>45950.507307974534</v>
-      </c>
-      <c r="G22" s="27"/>
+        <v>45950.520298958334</v>
+      </c>
+      <c r="G22" s="27">
+        <v>46033</v>
+      </c>
       <c r="H22" s="26" t="s">
         <v>91</v>
       </c>
@@ -3496,10 +3486,10 @@
         <v>117</v>
       </c>
       <c r="K22" s="26" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="L22" s="26" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M22" s="26">
         <v>0</v>
@@ -3519,7 +3509,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="26" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>88</v>
@@ -3528,15 +3518,17 @@
         <v>89</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="E23" s="27">
-        <v>45950.519731238426</v>
+        <v>45950.520432638892</v>
       </c>
       <c r="F23" s="27">
-        <v>45950.519731238426</v>
-      </c>
-      <c r="G23" s="27"/>
+        <v>45950.520432638892</v>
+      </c>
+      <c r="G23" s="27">
+        <v>46034</v>
+      </c>
       <c r="H23" s="26" t="s">
         <v>91</v>
       </c>
@@ -3547,10 +3539,10 @@
         <v>117</v>
       </c>
       <c r="K23" s="26" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="L23" s="26" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="M23" s="26">
         <v>0</v>
@@ -3568,238 +3560,94 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="27">
-        <v>45950.519979537035</v>
-      </c>
-      <c r="F24" s="27">
-        <v>45950.519979537035</v>
-      </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="J24" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="K24" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="L24" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="M24" s="26">
-        <v>0</v>
-      </c>
-      <c r="N24" s="26">
-        <v>0</v>
-      </c>
-      <c r="O24" s="26">
-        <v>0</v>
-      </c>
-      <c r="P24" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q24" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="E25" s="27">
-        <v>45950.520159583335</v>
-      </c>
-      <c r="F25" s="27">
-        <v>45950.520159583335</v>
-      </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="I25" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="K25" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="L25" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="M25" s="26">
-        <v>0</v>
-      </c>
-      <c r="N25" s="26">
-        <v>0</v>
-      </c>
-      <c r="O25" s="26">
-        <v>0</v>
-      </c>
-      <c r="P25" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q25" s="26">
-        <v>0</v>
-      </c>
-    </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="E26" s="27">
-        <v>45950.520298958334</v>
-      </c>
-      <c r="F26" s="27">
-        <v>45950.520298958334</v>
-      </c>
-      <c r="G26" s="27"/>
-      <c r="H26" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="I26" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="J26" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="K26" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="L26" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="M26" s="26">
-        <v>0</v>
-      </c>
-      <c r="N26" s="26">
-        <v>0</v>
-      </c>
-      <c r="O26" s="26">
-        <v>0</v>
-      </c>
-      <c r="P26" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q26" s="26">
-        <v>0</v>
+      <c r="B26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="27">
-        <v>45950.520432638892</v>
-      </c>
-      <c r="F27" s="27">
-        <v>45950.520432638892</v>
-      </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="J27" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="K27" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="L27" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="M27" s="26">
-        <v>0</v>
-      </c>
-      <c r="N27" s="26">
-        <v>0</v>
-      </c>
-      <c r="O27" s="26">
-        <v>0</v>
-      </c>
-      <c r="P27" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q27" s="26">
-        <v>0</v>
-      </c>
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="25">
+        <v>45936</v>
+      </c>
+      <c r="C27" s="25">
+        <v>45950</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="25">
+        <v>45950</v>
+      </c>
+      <c r="C28" s="25">
+        <v>45961</v>
+      </c>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="25">
+        <v>45961</v>
+      </c>
+      <c r="C29" s="25">
+        <v>45975</v>
+      </c>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="B30" t="s">
-        <v>157</v>
-      </c>
-      <c r="C30" t="s">
-        <v>158</v>
-      </c>
+      <c r="A30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="25">
+        <v>45975</v>
+      </c>
+      <c r="C30" s="25">
+        <v>45990</v>
+      </c>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="B31" s="25">
-        <v>45936</v>
+        <v>45990</v>
       </c>
       <c r="C31" s="25">
-        <v>45950</v>
-      </c>
+        <v>46005</v>
+      </c>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B32" s="25">
-        <v>45950</v>
+        <v>46005</v>
       </c>
       <c r="C32" s="25">
-        <v>45961</v>
+        <v>46021</v>
       </c>
       <c r="E32" s="25"/>
       <c r="F32" s="25"/>
@@ -3808,13 +3656,13 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B33" s="25">
-        <v>45961</v>
+        <v>46021</v>
       </c>
       <c r="C33" s="25">
-        <v>45975</v>
+        <v>46028</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="25"/>
@@ -3822,70 +3670,10 @@
       <c r="K33" s="25"/>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" s="25">
-        <v>45975</v>
-      </c>
-      <c r="C34" s="25">
-        <v>45990</v>
-      </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" s="25">
-        <v>45990</v>
-      </c>
-      <c r="C35" s="25">
-        <v>46005</v>
-      </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>143</v>
-      </c>
-      <c r="B36" s="25">
-        <v>46005</v>
-      </c>
-      <c r="C36" s="25">
-        <v>46021</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" t="s">
-        <v>148</v>
-      </c>
-      <c r="B37" s="25">
-        <v>46021</v>
-      </c>
-      <c r="C37" s="25">
-        <v>46028</v>
-      </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{5866E5C1-172E-4782-AFD1-E9BEE95982AD}">

</xml_diff>